<commit_message>
Final Features for Demo, Diab, BodyMeas
Finalized feature selections and renaming for Demographic, Diabetes, and BodyMeasures (FeatureMapping and Tableau Prep Flow changes)
</commit_message>
<xml_diff>
--- a/Data/FeatureMappings.xlsx
+++ b/Data/FeatureMappings.xlsx
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="312">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1088,6 +1088,12 @@
   </si>
   <si>
     <t>Polycystic ovarian syndrome - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</t>
+  </si>
+  <si>
+    <t>FAM_Income_Poverty_Ratio</t>
+  </si>
+  <si>
+    <t>Doctor_Visits_12Months</t>
   </si>
 </sst>
 </file>
@@ -1496,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2464,7 +2470,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2498,9 +2504,11 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>INDFMPIR (Type: numerical) - A ratio of family income to poverty guidelines.</v>
-      </c>
-      <c r="L26" s="3"/>
+        <v>FAM_Income_Poverty_Ratio (Type: numerical) - A ratio of family income to poverty guidelines.</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" t="str">
@@ -3365,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="E54" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3528,7 +3536,10 @@
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>DID250 (Type: numerical) - How many times {have you/has SP} seen this doctor or other health professional in the past 12 months?</v>
+        <v>Doctor_Visits_12Months (Type: numerical) - How many times {have you/has SP} seen this doctor or other health professional in the past 12 months?</v>
+      </c>
+      <c r="L4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added Glucose and HealthInsurance Data
Glucose and HealthInsurance NHANES tables were joined with the other datasets
</commit_message>
<xml_diff>
--- a/Data/FeatureMappings.xlsx
+++ b/Data/FeatureMappings.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="3070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="3070" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
     <sheet name="DEMO_J" sheetId="1" r:id="rId2"/>
     <sheet name="DIQ_J" sheetId="3" r:id="rId3"/>
     <sheet name="BMX_J" sheetId="4" r:id="rId4"/>
+    <sheet name="GLU_J" sheetId="7" r:id="rId5"/>
+    <sheet name="HIQ_J" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913" iterate="1" iterateCount="1"/>
   <extLst>
@@ -158,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="359">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1094,6 +1096,147 @@
   </si>
   <si>
     <t>Doctor_Visits_12Months</t>
+  </si>
+  <si>
+    <t>LBDGLUSI</t>
+  </si>
+  <si>
+    <t>Fasting Glucose (mmol/L)</t>
+  </si>
+  <si>
+    <t>GLU_J</t>
+  </si>
+  <si>
+    <t>Plasma Fasting Glucose</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>LBXGLU</t>
+  </si>
+  <si>
+    <t>Fasting Glucose (mg/dL)</t>
+  </si>
+  <si>
+    <t>Respondent sequence number</t>
+  </si>
+  <si>
+    <t>WTSAF2YR</t>
+  </si>
+  <si>
+    <t>Fasting Subsample 2 Year MEC Weight</t>
+  </si>
+  <si>
+    <t>Fasting_Glucose</t>
+  </si>
+  <si>
+    <t>HIQ011</t>
+  </si>
+  <si>
+    <t>The (first/next) questions are about health insurance. {Are you/Is SP} covered by health insurance or some other kind of health care plan? [Include health insurance obtained through employment or purchased directly as well as government programs like Medicare and Medicaid that provide medical care or help pay medical bills.]</t>
+  </si>
+  <si>
+    <t>HIQ_I</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>HIQ031A</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by private insurance?</t>
+  </si>
+  <si>
+    <t>HIQ031AA</t>
+  </si>
+  <si>
+    <t>No coverage of any type.</t>
+  </si>
+  <si>
+    <t>HIQ031B</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by Medicare?</t>
+  </si>
+  <si>
+    <t>HIQ031C</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by Medi-Gap?</t>
+  </si>
+  <si>
+    <t>HIQ031D</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by Medicaid?</t>
+  </si>
+  <si>
+    <t>HIQ031E</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by SCHIP (State Children's Health Insurance Program)?</t>
+  </si>
+  <si>
+    <t>HIQ031F</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by military health plan (Tricare/VA/Champ-VA)?</t>
+  </si>
+  <si>
+    <t>HIQ031G</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by Indian Health Service?</t>
+  </si>
+  <si>
+    <t>HIQ031H</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by state-sponsored health plan?</t>
+  </si>
+  <si>
+    <t>HIQ031I</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by other government insurance?</t>
+  </si>
+  <si>
+    <t>HIQ031J</t>
+  </si>
+  <si>
+    <t>{Are you/Is SP} covered by any single service plan?</t>
+  </si>
+  <si>
+    <t>HIQ105</t>
+  </si>
+  <si>
+    <t>Insurance card available or not.</t>
+  </si>
+  <si>
+    <t>HIQ210</t>
+  </si>
+  <si>
+    <t>In the past 12 months, was there any time when {you/SP} did not have any health insurance coverage?</t>
+  </si>
+  <si>
+    <t>HIQ260</t>
+  </si>
+  <si>
+    <t>{Do you/Does SP} have Medicare?</t>
+  </si>
+  <si>
+    <t>HIQ270</t>
+  </si>
+  <si>
+    <t>{Does this plan/Do any of these plans} cover any part of the cost of prescriptions?</t>
+  </si>
+  <si>
+    <t>Health_Insurance</t>
+  </si>
+  <si>
+    <t>Private_Insurance</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -5464,7 +5607,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K27"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6357,4 +6500,749 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2">
+        <v>2017</v>
+      </c>
+      <c r="H2">
+        <v>2018</v>
+      </c>
+      <c r="I2" t="s">
+        <v>316</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G3">
+        <v>2017</v>
+      </c>
+      <c r="H3">
+        <v>2018</v>
+      </c>
+      <c r="I3" t="s">
+        <v>316</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3" si="0">IF(ISBLANK(L3),CONCATENATE(C3, " (Type: numerical) - ", D3),CONCATENATE(L3, " (Type: numerical) - ", D3))</f>
+        <v>Fasting_Glucose (Type: numerical) - Fasting Glucose (mg/dL)</v>
+      </c>
+      <c r="L3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F4" t="s">
+        <v>315</v>
+      </c>
+      <c r="G4">
+        <v>2017</v>
+      </c>
+      <c r="H4">
+        <v>2018</v>
+      </c>
+      <c r="I4" t="s">
+        <v>316</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G5">
+        <v>2017</v>
+      </c>
+      <c r="H5">
+        <v>2018</v>
+      </c>
+      <c r="I5" t="s">
+        <v>316</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2">
+        <v>2015</v>
+      </c>
+      <c r="H2">
+        <v>2016</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K18" si="0">IF(ISBLANK(L2),CONCATENATE(C2, " (Type: numerical) - ", D2),CONCATENATE(L2, " (Type: numerical) - ", D2))</f>
+        <v>Health_Insurance (Type: numerical) - The (first/next) questions are about health insurance. {Are you/Is SP} covered by health insurance or some other kind of health care plan? [Include health insurance obtained through employment or purchased directly as well as government programs like Medicare and Medicaid that provide medical care or help pay medical bills.]</v>
+      </c>
+      <c r="L2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G3">
+        <v>2015</v>
+      </c>
+      <c r="H3">
+        <v>2016</v>
+      </c>
+      <c r="I3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="0"/>
+        <v>Private_Insurance (Type: numerical) - {Are you/Is SP} covered by private insurance?</v>
+      </c>
+      <c r="L3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F4" t="s">
+        <v>326</v>
+      </c>
+      <c r="G4">
+        <v>2015</v>
+      </c>
+      <c r="H4">
+        <v>2016</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031AA (Type: numerical) - No coverage of any type.</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" t="s">
+        <v>325</v>
+      </c>
+      <c r="F5" t="s">
+        <v>326</v>
+      </c>
+      <c r="G5">
+        <v>2015</v>
+      </c>
+      <c r="H5">
+        <v>2016</v>
+      </c>
+      <c r="I5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031B (Type: numerical) - {Are you/Is SP} covered by Medicare?</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E6" t="s">
+        <v>325</v>
+      </c>
+      <c r="F6" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6">
+        <v>2015</v>
+      </c>
+      <c r="H6">
+        <v>2016</v>
+      </c>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031C (Type: numerical) - {Are you/Is SP} covered by Medi-Gap?</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" t="s">
+        <v>325</v>
+      </c>
+      <c r="F7" t="s">
+        <v>326</v>
+      </c>
+      <c r="G7">
+        <v>2015</v>
+      </c>
+      <c r="H7">
+        <v>2016</v>
+      </c>
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031D (Type: numerical) - {Are you/Is SP} covered by Medicaid?</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8" t="s">
+        <v>325</v>
+      </c>
+      <c r="F8" t="s">
+        <v>326</v>
+      </c>
+      <c r="G8">
+        <v>2015</v>
+      </c>
+      <c r="H8">
+        <v>2016</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031E (Type: numerical) - {Are you/Is SP} covered by SCHIP (State Children's Health Insurance Program)?</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" t="s">
+        <v>326</v>
+      </c>
+      <c r="G9">
+        <v>2015</v>
+      </c>
+      <c r="H9">
+        <v>2016</v>
+      </c>
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031F (Type: numerical) - {Are you/Is SP} covered by military health plan (Tricare/VA/Champ-VA)?</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" t="s">
+        <v>342</v>
+      </c>
+      <c r="E10" t="s">
+        <v>325</v>
+      </c>
+      <c r="F10" t="s">
+        <v>326</v>
+      </c>
+      <c r="G10">
+        <v>2015</v>
+      </c>
+      <c r="H10">
+        <v>2016</v>
+      </c>
+      <c r="I10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031G (Type: numerical) - {Are you/Is SP} covered by Indian Health Service?</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E11" t="s">
+        <v>325</v>
+      </c>
+      <c r="F11" t="s">
+        <v>326</v>
+      </c>
+      <c r="G11">
+        <v>2015</v>
+      </c>
+      <c r="H11">
+        <v>2016</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031H (Type: numerical) - {Are you/Is SP} covered by state-sponsored health plan?</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" t="s">
+        <v>326</v>
+      </c>
+      <c r="G12">
+        <v>2015</v>
+      </c>
+      <c r="H12">
+        <v>2016</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031I (Type: numerical) - {Are you/Is SP} covered by other government insurance?</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F13" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13">
+        <v>2015</v>
+      </c>
+      <c r="H13">
+        <v>2016</v>
+      </c>
+      <c r="I13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ031J (Type: numerical) - {Are you/Is SP} covered by any single service plan?</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E14" t="s">
+        <v>325</v>
+      </c>
+      <c r="F14" t="s">
+        <v>326</v>
+      </c>
+      <c r="G14">
+        <v>2015</v>
+      </c>
+      <c r="H14">
+        <v>2016</v>
+      </c>
+      <c r="I14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ105 (Type: numerical) - Insurance card available or not.</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>351</v>
+      </c>
+      <c r="D15" t="s">
+        <v>352</v>
+      </c>
+      <c r="E15" t="s">
+        <v>325</v>
+      </c>
+      <c r="F15" t="s">
+        <v>326</v>
+      </c>
+      <c r="G15">
+        <v>2015</v>
+      </c>
+      <c r="H15">
+        <v>2016</v>
+      </c>
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ210 (Type: numerical) - In the past 12 months, was there any time when {you/SP} did not have any health insurance coverage?</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>353</v>
+      </c>
+      <c r="D16" t="s">
+        <v>354</v>
+      </c>
+      <c r="E16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F16" t="s">
+        <v>326</v>
+      </c>
+      <c r="G16">
+        <v>2015</v>
+      </c>
+      <c r="H16">
+        <v>2016</v>
+      </c>
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ260 (Type: numerical) - {Do you/Does SP} have Medicare?</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>355</v>
+      </c>
+      <c r="D17" t="s">
+        <v>356</v>
+      </c>
+      <c r="E17" t="s">
+        <v>325</v>
+      </c>
+      <c r="F17" t="s">
+        <v>326</v>
+      </c>
+      <c r="G17">
+        <v>2015</v>
+      </c>
+      <c r="H17">
+        <v>2016</v>
+      </c>
+      <c r="I17" t="s">
+        <v>114</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>HIQ270 (Type: numerical) - {Does this plan/Do any of these plans} cover any part of the cost of prescriptions?</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18" t="s">
+        <v>326</v>
+      </c>
+      <c r="G18">
+        <v>2015</v>
+      </c>
+      <c r="H18">
+        <v>2016</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>SEQN (Type: numerical) - Respondent sequence number.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding A1c data and CSVs
Added A1c join to Tableau Prep, generated new NHANES Data table, and added CSVs to file
</commit_message>
<xml_diff>
--- a/Data/FeatureMappings.xlsx
+++ b/Data/FeatureMappings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\OneDrive\Documents\GitHub\DAEN-690-Capstone-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prahi\Desktop\DAEN 690 - Capstone\Final Project - GitHub Repo\DAEN-690-Capstone-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815A4836-0E8C-4A54-B49F-2DEF52BCD981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="3070" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -18,23 +19,33 @@
     <sheet name="BMX_J" sheetId="4" r:id="rId4"/>
     <sheet name="GLU_J" sheetId="7" r:id="rId5"/>
     <sheet name="HIQ_J" sheetId="8" r:id="rId6"/>
+    <sheet name="Glycohemoglobin" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateCount="1"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Johnny Ha</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -160,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="367">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1243,13 +1254,31 @@
   </si>
   <si>
     <t>Len_Recum</t>
+  </si>
+  <si>
+    <t>Glycohemoglobin 2017-2018/Glycohemoglobin 2015-2016</t>
+  </si>
+  <si>
+    <t>LBXGH</t>
+  </si>
+  <si>
+    <t>Glycohemoglobin (%)</t>
+  </si>
+  <si>
+    <t>Glycohemoglobin 2017-2018/Glycohemoglobin 2015-2017</t>
+  </si>
+  <si>
+    <t>A1c</t>
+  </si>
+  <si>
+    <t>A1c (Type: numerical) - Glycohemoglobin (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1269,6 +1298,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1603,44 +1638,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -1651,30 +1686,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.81640625" customWidth="1"/>
-    <col min="12" max="12" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -1709,7 +1744,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(B2=C2, "Yes","No")</f>
         <v>Yes</v>
@@ -1747,7 +1782,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A48" si="0">IF(B3=C3, "Yes","No")</f>
         <v>Yes</v>
@@ -1787,7 +1822,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1827,7 +1862,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1867,7 +1902,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1907,7 +1942,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1945,7 +1980,7 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1985,7 +2020,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2023,7 +2058,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2061,7 +2096,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2099,7 +2134,7 @@
       </c>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2139,7 +2174,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2148,7 +2183,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2188,7 +2223,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2228,7 +2263,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2268,7 +2303,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2308,7 +2343,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2348,7 +2383,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2388,7 +2423,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2428,7 +2463,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2468,7 +2503,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2506,7 +2541,7 @@
       </c>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2544,7 +2579,7 @@
       </c>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2582,7 +2617,7 @@
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2622,7 +2657,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2662,7 +2697,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2702,7 +2737,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2740,7 +2775,7 @@
       </c>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2778,7 +2813,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2816,7 +2851,7 @@
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2856,7 +2891,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2894,7 +2929,7 @@
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2934,7 +2969,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2972,7 +3007,7 @@
       </c>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3012,7 +3047,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3050,7 +3085,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3088,7 +3123,7 @@
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3128,7 +3163,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3166,7 +3201,7 @@
       </c>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3204,7 +3239,7 @@
       </c>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3242,7 +3277,7 @@
       </c>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3280,7 +3315,7 @@
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3318,7 +3353,7 @@
       </c>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3356,7 +3391,7 @@
       </c>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3396,7 +3431,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3434,7 +3469,7 @@
       </c>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3474,7 +3509,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3522,30 +3557,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="95.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19.36328125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -3580,7 +3615,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(B2=C2, "yes","no")</f>
         <v>yes</v>
@@ -3617,7 +3652,7 @@
         <v>DID040 (Type: numerical) - How old {was SP/were you} when a doctor or other health professional first told {you/him/her} that {you/he/she} had diabetes or sugar diabetes?</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A55" si="0">IF(B3=C3, "yes","no")</f>
         <v>yes</v>
@@ -3654,7 +3689,7 @@
         <v>DID060 (Type: numerical) - For how long {have you/has SP} been taking insulin?</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3694,7 +3729,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3731,7 +3766,7 @@
         <v>DID260 (Type: numerical) - How often {do you check your/does SP check his/her} blood for glucose or sugar? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3768,7 +3803,7 @@
         <v>DID310D (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} blood pressure should be?</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3805,7 +3840,7 @@
         <v>DID310S (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} blood pressure should be?</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3842,7 +3877,7 @@
         <v>DID320 (Type: numerical) - One part of total serum cholesterol in {your/SP's} blood is a bad cholesterol, called LDL, which builds up and clogs {your/his/her} arteries. What was {your/his/her} most recent LDL cholesterol number?</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3879,7 +3914,7 @@
         <v>DID330 (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} LDL cholesterol should be?</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3916,7 +3951,7 @@
         <v>DID341 (Type: numerical) - During the past 12 months, about how many times has a doctor or other health professional checked {your/SP's} feet for any sores or irritations?</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3953,7 +3988,7 @@
         <v>DID350 (Type: numerical) - How often {do you check your feet/does SP check (his/her) feet} for sores or irritations? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3993,7 +4028,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4033,7 +4068,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4070,7 +4105,7 @@
         <v>DIQ060U (Type: numerical) - UNIT OF MEASURE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4110,7 +4145,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4147,7 +4182,7 @@
         <v>DIQ080 (Type: numerical) - Has a doctor ever told {you/SP} that diabetes has affected {your/his/her} eyes or that {you/s/he} had retinopathy (ret-in-op-ath-ee)?</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4187,7 +4222,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4227,7 +4262,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4264,7 +4299,7 @@
         <v>DIQ172 (Type: numerical) - {Do you/Does SP} feel {you/he/she} could be at risk for diabetes or prediabetes?</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4304,7 +4339,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4344,7 +4379,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4381,7 +4416,7 @@
         <v>DIQ175C (Type: numerical) - Age - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4418,7 +4453,7 @@
         <v>DIQ175D (Type: numerical) - Poor Diet - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4455,7 +4490,7 @@
         <v>DIQ175E (Type: numerical) - Race - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4492,7 +4527,7 @@
         <v>DIQ175F (Type: numerical) - Had a baby weighed over 9 lbs. at birth - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4529,7 +4564,7 @@
         <v>DIQ175G (Type: numerical) - Lack of physical activity - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4566,7 +4601,7 @@
         <v>DIQ175H (Type: numerical) - High blood pressure - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4603,7 +4638,7 @@
         <v>DIQ175I (Type: numerical) - High blood sugar - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4640,7 +4675,7 @@
         <v>DIQ175J (Type: numerical) - High cholesterol - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4677,7 +4712,7 @@
         <v>DIQ175K (Type: numerical) - Hypoglycemic - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4714,7 +4749,7 @@
         <v>DIQ175L (Type: numerical) - Extreme Hunger - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4751,7 +4786,7 @@
         <v>DIQ175M (Type: numerical) - Tingling/numbness in hands or feet - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4788,7 +4823,7 @@
         <v>DIQ175N (Type: numerical) - Blurred vision - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4825,7 +4860,7 @@
         <v>DIQ175O (Type: numerical) - Increased Fatigue - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4862,7 +4897,7 @@
         <v>DIQ175P (Type: numerical) - Anyone could be at risk - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4899,7 +4934,7 @@
         <v>DIQ175Q (Type: numerical) - Doctor warning - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4936,7 +4971,7 @@
         <v>DIQ175R (Type: numerical) - Other, specify - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4973,7 +5008,7 @@
         <v>DIQ175S (Type: numerical) - Gestational diabetes - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5010,7 +5045,7 @@
         <v>DIQ175T (Type: numerical) - Frequent urination - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5047,7 +5082,7 @@
         <v>DIQ175U (Type: numerical) - Thirst - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5084,7 +5119,7 @@
         <v>DIQ175V (Type: numerical) - Craving for sweet/eating a lot of sugar - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes?</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5121,7 +5156,7 @@
         <v>DIQ175W (Type: numerical) - Medication - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5158,7 +5193,7 @@
         <v>DIQ175X (Type: numerical) - Polycystic ovarian syndrome - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5198,7 +5233,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5235,7 +5270,7 @@
         <v>DIQ230 (Type: numerical) - When was the last time {you/SP} saw a diabetes nurse educator or dietitian or nutritionist for {your/his/her} diabetes? Do not include doctors or other health professionals.</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5272,7 +5307,7 @@
         <v>DIQ240 (Type: numerical) - Is there one doctor or other health professional {you usually see/SP usually sees} for {your/his/her} diabetes? Do not include specialists to whom {you have/SP has} been referred such as diabetes educators, dieticians or foot and eye doctors.</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5309,7 +5344,7 @@
         <v>DIQ260U (Type: numerical) - How often {do you check your/does SP check his/her} blood for glucose or sugar? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5346,7 +5381,7 @@
         <v>DIQ275 (Type: numerical) - Glycosylated (GLY-KOH-SIH-LAY-TED) hemoglobin or the "A one C" test measures your average level of blood sugar for the past 3 months, and usually ranges between 5.0 and 13.9. During the past 12 months, has a doctor or other health professional checked {your/SP's} glycosylated hemoglobin or "A one C"?</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5383,7 +5418,7 @@
         <v>DIQ280 (Type: numerical) - What was {your/SP's} last "A one C" level?</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5420,7 +5455,7 @@
         <v>DIQ291 (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} "A one C" level should be? (Pick the lowest level recommended by your health care professional.)</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5457,7 +5492,7 @@
         <v>DIQ300D (Type: numerical) - Blood pressure is usually given as one number over another. What was {your/SP's} most recent blood pressure in numbers?</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5494,7 +5529,7 @@
         <v>DIQ300S (Type: numerical) - Blood pressure is usually given as one number over another. What was {your/SP's} most recent blood pressure in numbers?</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5531,7 +5566,7 @@
         <v>DIQ350U (Type: numerical) - How often {do you check your feet/does SP check (his/her) feet} for sores or irritations? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5568,7 +5603,7 @@
         <v>DIQ360 (Type: numerical) - When was the last time {you/SP} had an eye exam in which the pupils were dilated? This would have made {you/SP} temporarily sensitive to bright light.</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5612,30 +5647,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -5670,7 +5705,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(B2=C2, "yes", "no")</f>
         <v>no</v>
@@ -5679,7 +5714,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A27" si="0">IF(B3=C3, "yes", "no")</f>
         <v>no</v>
@@ -5688,7 +5723,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -5697,7 +5732,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5734,7 +5769,7 @@
         <v>BMDSTATS (Type: numerical) - Body Measures Component status Code</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5771,7 +5806,7 @@
         <v>BMIARMC (Type: numerical) - Arm Circumference Comment</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5808,7 +5843,7 @@
         <v>BMIARML (Type: numerical) - Upper Arm Length Comment</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5845,7 +5880,7 @@
         <v>BMIHEAD (Type: numerical) - Head Circumference Comment</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5882,7 +5917,7 @@
         <v>BMIHT (Type: numerical) - Standing Height Comment</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5919,7 +5954,7 @@
         <v>BMILEG (Type: numerical) - Upper Leg Length Comment</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5956,7 +5991,7 @@
         <v>BMIRECUM (Type: numerical) - Recumbent Length Comment</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5993,7 +6028,7 @@
         <v>BMIWAIST (Type: numerical) - Waist Circumference Comment</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6030,7 +6065,7 @@
         <v>BMIWT (Type: numerical) - Weight Comment</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6070,7 +6105,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6110,7 +6145,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6150,7 +6185,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6190,7 +6225,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6230,7 +6265,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6270,7 +6305,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6310,7 +6345,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6343,7 +6378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6376,7 +6411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6385,7 +6420,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6394,7 +6429,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6434,7 +6469,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6474,7 +6509,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6518,27 +6553,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="84.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -6570,7 +6605,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>312</v>
       </c>
@@ -6596,7 +6631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>317</v>
       </c>
@@ -6629,7 +6664,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>91</v>
       </c>
@@ -6655,7 +6690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>320</v>
       </c>
@@ -6688,27 +6723,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -6740,7 +6776,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>323</v>
       </c>
@@ -6773,7 +6809,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>327</v>
       </c>
@@ -6806,7 +6842,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>329</v>
       </c>
@@ -6836,7 +6872,7 @@
         <v>HIQ031AA (Type: numerical) - No coverage of any type.</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>331</v>
       </c>
@@ -6866,7 +6902,7 @@
         <v>HIQ031B (Type: numerical) - {Are you/Is SP} covered by Medicare?</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>333</v>
       </c>
@@ -6896,7 +6932,7 @@
         <v>HIQ031C (Type: numerical) - {Are you/Is SP} covered by Medi-Gap?</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>335</v>
       </c>
@@ -6926,7 +6962,7 @@
         <v>HIQ031D (Type: numerical) - {Are you/Is SP} covered by Medicaid?</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>337</v>
       </c>
@@ -6956,7 +6992,7 @@
         <v>HIQ031E (Type: numerical) - {Are you/Is SP} covered by SCHIP (State Children's Health Insurance Program)?</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>339</v>
       </c>
@@ -6986,7 +7022,7 @@
         <v>HIQ031F (Type: numerical) - {Are you/Is SP} covered by military health plan (Tricare/VA/Champ-VA)?</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>341</v>
       </c>
@@ -7016,7 +7052,7 @@
         <v>HIQ031G (Type: numerical) - {Are you/Is SP} covered by Indian Health Service?</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>343</v>
       </c>
@@ -7046,7 +7082,7 @@
         <v>HIQ031H (Type: numerical) - {Are you/Is SP} covered by state-sponsored health plan?</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>345</v>
       </c>
@@ -7076,7 +7112,7 @@
         <v>HIQ031I (Type: numerical) - {Are you/Is SP} covered by other government insurance?</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>347</v>
       </c>
@@ -7106,7 +7142,7 @@
         <v>HIQ031J (Type: numerical) - {Are you/Is SP} covered by any single service plan?</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>349</v>
       </c>
@@ -7136,7 +7172,7 @@
         <v>HIQ105 (Type: numerical) - Insurance card available or not.</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>351</v>
       </c>
@@ -7166,7 +7202,7 @@
         <v>HIQ210 (Type: numerical) - In the past 12 months, was there any time when {you/SP} did not have any health insurance coverage?</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>353</v>
       </c>
@@ -7196,7 +7232,7 @@
         <v>HIQ260 (Type: numerical) - {Do you/Does SP} have Medicare?</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>355</v>
       </c>
@@ -7226,7 +7262,7 @@
         <v>HIQ270 (Type: numerical) - {Does this plan/Do any of these plans} cover any part of the cost of prescriptions?</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>91</v>
       </c>
@@ -7260,4 +7296,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5FE21F-9D84-4A68-94F4-21A85F04D6D5}">
+  <dimension ref="C1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G2">
+        <v>2015</v>
+      </c>
+      <c r="H2">
+        <v>2018</v>
+      </c>
+      <c r="I2" t="s">
+        <v>316</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3">
+        <v>2015</v>
+      </c>
+      <c r="H3">
+        <v>2018</v>
+      </c>
+      <c r="I3" t="s">
+        <v>316</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>366</v>
+      </c>
+      <c r="L3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Packaged Tableau Prep Flow
Packaged Tableau Prep Flow
</commit_message>
<xml_diff>
--- a/Data/FeatureMappings.xlsx
+++ b/Data/FeatureMappings.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prahi\Desktop\DAEN 690 - Capstone\Final Project - GitHub Repo\DAEN-690-Capstone-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\OneDrive\Documents\GitHub\DAEN-690-Capstone-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815A4836-0E8C-4A54-B49F-2DEF52BCD981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -40,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Johnny Ha</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1277,7 +1276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1638,44 +1637,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -1686,30 +1685,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -1744,7 +1743,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="str">
         <f>IF(B2=C2, "Yes","No")</f>
         <v>Yes</v>
@@ -1782,7 +1781,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A48" si="0">IF(B3=C3, "Yes","No")</f>
         <v>Yes</v>
@@ -1822,7 +1821,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1862,7 +1861,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1902,7 +1901,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1942,7 +1941,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -1980,7 +1979,7 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2020,7 +2019,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2058,7 +2057,7 @@
       </c>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2096,7 +2095,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2134,7 +2133,7 @@
       </c>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2174,7 +2173,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2183,7 +2182,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2223,7 +2222,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2263,7 +2262,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2303,7 +2302,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>No</v>
@@ -2343,7 +2342,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2383,7 +2382,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2423,7 +2422,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2463,7 +2462,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2503,7 +2502,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2541,7 +2540,7 @@
       </c>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2579,7 +2578,7 @@
       </c>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2617,7 +2616,7 @@
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2657,7 +2656,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2697,7 +2696,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2737,7 +2736,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2775,7 +2774,7 @@
       </c>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2813,7 +2812,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2851,7 +2850,7 @@
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2891,7 +2890,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2929,7 +2928,7 @@
       </c>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -2969,7 +2968,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3007,7 +3006,7 @@
       </c>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3047,7 +3046,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3085,7 +3084,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3123,7 +3122,7 @@
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3163,7 +3162,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3201,7 +3200,7 @@
       </c>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3239,7 +3238,7 @@
       </c>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3277,7 +3276,7 @@
       </c>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3315,7 +3314,7 @@
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3353,7 +3352,7 @@
       </c>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3391,7 +3390,7 @@
       </c>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3431,7 +3430,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3469,7 +3468,7 @@
       </c>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3509,7 +3508,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Yes</v>
@@ -3557,30 +3556,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="95.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="95.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>IF(B2=C2, "yes","no")</f>
         <v>yes</v>
@@ -3652,7 +3651,7 @@
         <v>DID040 (Type: numerical) - How old {was SP/were you} when a doctor or other health professional first told {you/him/her} that {you/he/she} had diabetes or sugar diabetes?</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A55" si="0">IF(B3=C3, "yes","no")</f>
         <v>yes</v>
@@ -3689,7 +3688,7 @@
         <v>DID060 (Type: numerical) - For how long {have you/has SP} been taking insulin?</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3729,7 +3728,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3766,7 +3765,7 @@
         <v>DID260 (Type: numerical) - How often {do you check your/does SP check his/her} blood for glucose or sugar? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3803,7 +3802,7 @@
         <v>DID310D (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} blood pressure should be?</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3840,7 +3839,7 @@
         <v>DID310S (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} blood pressure should be?</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3877,7 +3876,7 @@
         <v>DID320 (Type: numerical) - One part of total serum cholesterol in {your/SP's} blood is a bad cholesterol, called LDL, which builds up and clogs {your/his/her} arteries. What was {your/his/her} most recent LDL cholesterol number?</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3914,7 +3913,7 @@
         <v>DID330 (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} LDL cholesterol should be?</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3951,7 +3950,7 @@
         <v>DID341 (Type: numerical) - During the past 12 months, about how many times has a doctor or other health professional checked {your/SP's} feet for any sores or irritations?</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -3988,7 +3987,7 @@
         <v>DID350 (Type: numerical) - How often {do you check your feet/does SP check (his/her) feet} for sores or irritations? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4028,7 +4027,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4068,7 +4067,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4105,7 +4104,7 @@
         <v>DIQ060U (Type: numerical) - UNIT OF MEASURE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4145,7 +4144,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4182,7 +4181,7 @@
         <v>DIQ080 (Type: numerical) - Has a doctor ever told {you/SP} that diabetes has affected {your/his/her} eyes or that {you/s/he} had retinopathy (ret-in-op-ath-ee)?</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4222,7 +4221,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4262,7 +4261,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4299,7 +4298,7 @@
         <v>DIQ172 (Type: numerical) - {Do you/Does SP} feel {you/he/she} could be at risk for diabetes or prediabetes?</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4339,7 +4338,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4379,7 +4378,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4416,7 +4415,7 @@
         <v>DIQ175C (Type: numerical) - Age - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4453,7 +4452,7 @@
         <v>DIQ175D (Type: numerical) - Poor Diet - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4490,7 +4489,7 @@
         <v>DIQ175E (Type: numerical) - Race - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4527,7 +4526,7 @@
         <v>DIQ175F (Type: numerical) - Had a baby weighed over 9 lbs. at birth - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4564,7 +4563,7 @@
         <v>DIQ175G (Type: numerical) - Lack of physical activity - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4601,7 +4600,7 @@
         <v>DIQ175H (Type: numerical) - High blood pressure - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4638,7 +4637,7 @@
         <v>DIQ175I (Type: numerical) - High blood sugar - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4675,7 +4674,7 @@
         <v>DIQ175J (Type: numerical) - High cholesterol - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4712,7 +4711,7 @@
         <v>DIQ175K (Type: numerical) - Hypoglycemic - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4749,7 +4748,7 @@
         <v>DIQ175L (Type: numerical) - Extreme Hunger - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4786,7 +4785,7 @@
         <v>DIQ175M (Type: numerical) - Tingling/numbness in hands or feet - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4823,7 +4822,7 @@
         <v>DIQ175N (Type: numerical) - Blurred vision - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4860,7 +4859,7 @@
         <v>DIQ175O (Type: numerical) - Increased Fatigue - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4897,7 +4896,7 @@
         <v>DIQ175P (Type: numerical) - Anyone could be at risk - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4934,7 +4933,7 @@
         <v>DIQ175Q (Type: numerical) - Doctor warning - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -4971,7 +4970,7 @@
         <v>DIQ175R (Type: numerical) - Other, specify - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5008,7 +5007,7 @@
         <v>DIQ175S (Type: numerical) - Gestational diabetes - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5045,7 +5044,7 @@
         <v>DIQ175T (Type: numerical) - Frequent urination - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5082,7 +5081,7 @@
         <v>DIQ175U (Type: numerical) - Thirst - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5119,7 +5118,7 @@
         <v>DIQ175V (Type: numerical) - Craving for sweet/eating a lot of sugar - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes?</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5156,7 +5155,7 @@
         <v>DIQ175W (Type: numerical) - Medication - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5193,7 +5192,7 @@
         <v>DIQ175X (Type: numerical) - Polycystic ovarian syndrome - Why {Do you/Does SP} think {you are/he is/she is} at risk for diabetes or prediabetes? [Anything else?]</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5233,7 +5232,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5270,7 +5269,7 @@
         <v>DIQ230 (Type: numerical) - When was the last time {you/SP} saw a diabetes nurse educator or dietitian or nutritionist for {your/his/her} diabetes? Do not include doctors or other health professionals.</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5307,7 +5306,7 @@
         <v>DIQ240 (Type: numerical) - Is there one doctor or other health professional {you usually see/SP usually sees} for {your/his/her} diabetes? Do not include specialists to whom {you have/SP has} been referred such as diabetes educators, dieticians or foot and eye doctors.</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5344,7 +5343,7 @@
         <v>DIQ260U (Type: numerical) - How often {do you check your/does SP check his/her} blood for glucose or sugar? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5381,7 +5380,7 @@
         <v>DIQ275 (Type: numerical) - Glycosylated (GLY-KOH-SIH-LAY-TED) hemoglobin or the "A one C" test measures your average level of blood sugar for the past 3 months, and usually ranges between 5.0 and 13.9. During the past 12 months, has a doctor or other health professional checked {your/SP's} glycosylated hemoglobin or "A one C"?</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5418,7 +5417,7 @@
         <v>DIQ280 (Type: numerical) - What was {your/SP's} last "A one C" level?</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5455,7 +5454,7 @@
         <v>DIQ291 (Type: numerical) - What does {your/SP's} doctor or other health professional say {your/his/her} "A one C" level should be? (Pick the lowest level recommended by your health care professional.)</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5492,7 +5491,7 @@
         <v>DIQ300D (Type: numerical) - Blood pressure is usually given as one number over another. What was {your/SP's} most recent blood pressure in numbers?</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5529,7 +5528,7 @@
         <v>DIQ300S (Type: numerical) - Blood pressure is usually given as one number over another. What was {your/SP's} most recent blood pressure in numbers?</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5566,7 +5565,7 @@
         <v>DIQ350U (Type: numerical) - How often {do you check your feet/does SP check (his/her) feet} for sores or irritations? Include times when checked by a family member or friend, but do not include times when checked by a doctor or other health professional.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5603,7 +5602,7 @@
         <v>DIQ360 (Type: numerical) - When was the last time {you/SP} had an eye exam in which the pupils were dilated? This would have made {you/SP} temporarily sensitive to bright light.</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5647,30 +5646,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>109</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>IF(B2=C2, "yes", "no")</f>
         <v>no</v>
@@ -5714,7 +5713,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A27" si="0">IF(B3=C3, "yes", "no")</f>
         <v>no</v>
@@ -5723,7 +5722,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -5732,7 +5731,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5769,7 +5768,7 @@
         <v>BMDSTATS (Type: numerical) - Body Measures Component status Code</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5806,7 +5805,7 @@
         <v>BMIARMC (Type: numerical) - Arm Circumference Comment</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5843,7 +5842,7 @@
         <v>BMIARML (Type: numerical) - Upper Arm Length Comment</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5880,7 +5879,7 @@
         <v>BMIHEAD (Type: numerical) - Head Circumference Comment</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5917,7 +5916,7 @@
         <v>BMIHT (Type: numerical) - Standing Height Comment</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5954,7 +5953,7 @@
         <v>BMILEG (Type: numerical) - Upper Leg Length Comment</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -5991,7 +5990,7 @@
         <v>BMIRECUM (Type: numerical) - Recumbent Length Comment</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6028,7 +6027,7 @@
         <v>BMIWAIST (Type: numerical) - Waist Circumference Comment</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6065,7 +6064,7 @@
         <v>BMIWT (Type: numerical) - Weight Comment</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6105,7 +6104,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6145,7 +6144,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6185,7 +6184,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6225,7 +6224,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6265,7 +6264,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6305,7 +6304,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6345,7 +6344,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6378,7 +6377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6411,7 +6410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6420,7 +6419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
@@ -6429,7 +6428,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6469,7 +6468,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6509,7 +6508,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>yes</v>
@@ -6553,27 +6552,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="84.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -6605,7 +6604,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>312</v>
       </c>
@@ -6631,7 +6630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>317</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>91</v>
       </c>
@@ -6690,7 +6689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>320</v>
       </c>
@@ -6723,28 +6722,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -6776,7 +6775,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>323</v>
       </c>
@@ -6809,7 +6808,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>327</v>
       </c>
@@ -6842,7 +6841,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>329</v>
       </c>
@@ -6872,7 +6871,7 @@
         <v>HIQ031AA (Type: numerical) - No coverage of any type.</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>331</v>
       </c>
@@ -6902,7 +6901,7 @@
         <v>HIQ031B (Type: numerical) - {Are you/Is SP} covered by Medicare?</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>333</v>
       </c>
@@ -6932,7 +6931,7 @@
         <v>HIQ031C (Type: numerical) - {Are you/Is SP} covered by Medi-Gap?</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>335</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>HIQ031D (Type: numerical) - {Are you/Is SP} covered by Medicaid?</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>337</v>
       </c>
@@ -6992,7 +6991,7 @@
         <v>HIQ031E (Type: numerical) - {Are you/Is SP} covered by SCHIP (State Children's Health Insurance Program)?</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>339</v>
       </c>
@@ -7022,7 +7021,7 @@
         <v>HIQ031F (Type: numerical) - {Are you/Is SP} covered by military health plan (Tricare/VA/Champ-VA)?</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>341</v>
       </c>
@@ -7052,7 +7051,7 @@
         <v>HIQ031G (Type: numerical) - {Are you/Is SP} covered by Indian Health Service?</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>343</v>
       </c>
@@ -7082,7 +7081,7 @@
         <v>HIQ031H (Type: numerical) - {Are you/Is SP} covered by state-sponsored health plan?</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>345</v>
       </c>
@@ -7112,7 +7111,7 @@
         <v>HIQ031I (Type: numerical) - {Are you/Is SP} covered by other government insurance?</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>347</v>
       </c>
@@ -7142,7 +7141,7 @@
         <v>HIQ031J (Type: numerical) - {Are you/Is SP} covered by any single service plan?</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>349</v>
       </c>
@@ -7172,7 +7171,7 @@
         <v>HIQ105 (Type: numerical) - Insurance card available or not.</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>351</v>
       </c>
@@ -7202,7 +7201,7 @@
         <v>HIQ210 (Type: numerical) - In the past 12 months, was there any time when {you/SP} did not have any health insurance coverage?</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>353</v>
       </c>
@@ -7232,7 +7231,7 @@
         <v>HIQ260 (Type: numerical) - {Do you/Does SP} have Medicare?</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>355</v>
       </c>
@@ -7262,7 +7261,7 @@
         <v>HIQ270 (Type: numerical) - {Does this plan/Do any of these plans} cover any part of the cost of prescriptions?</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>91</v>
       </c>
@@ -7299,28 +7298,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5FE21F-9D84-4A68-94F4-21A85F04D6D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -7352,7 +7351,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>91</v>
       </c>
@@ -7378,7 +7377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>362</v>
       </c>

</xml_diff>